<commit_message>
Pequenas alterações e testes...
</commit_message>
<xml_diff>
--- a/ratTrainer/sessions.xlsx
+++ b/ratTrainer/sessions.xlsx
@@ -1,84 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Desktop\repos\Projeto ratos\miceTrainer\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF26A58E-0C40-47AB-B0F7-AC595ED18488}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>VDS</t>
-  </si>
-  <si>
-    <t>Date started</t>
-  </si>
-  <si>
-    <t>Date Ended</t>
-  </si>
-  <si>
-    <t>Right Sensor Activations</t>
-  </si>
-  <si>
-    <t>Left Sensor Activations</t>
-  </si>
-  <si>
-    <t>Feeder Sensor Activations</t>
-  </si>
-  <si>
-    <t>Premature Responses</t>
-  </si>
-  <si>
-    <t>Omission Responses</t>
-  </si>
-  <si>
-    <t>Timed Responses</t>
-  </si>
-  <si>
-    <t>Perseverant Responses</t>
-  </si>
-  <si>
-    <t>Number of trials</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+  </numFmts>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -96,23 +55,83 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -412,65 +431,165 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" customWidth="1"/>
-    <col min="2" max="2" width="29.33203125" customWidth="1"/>
-    <col min="3" max="3" width="42" customWidth="1"/>
-    <col min="4" max="4" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.5546875" customWidth="1"/>
+    <col width="8.6640625" customWidth="1" min="1" max="1"/>
+    <col width="29.33203125" customWidth="1" min="2" max="2"/>
+    <col width="42" customWidth="1" min="3" max="3"/>
+    <col width="21.5546875" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="20.33203125" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="22.88671875" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="19.33203125" bestFit="1" customWidth="1" min="7" max="7"/>
+    <col width="18.109375" bestFit="1" customWidth="1" min="8" max="8"/>
+    <col width="15.5546875" bestFit="1" customWidth="1" min="9" max="9"/>
+    <col width="20.44140625" bestFit="1" customWidth="1" min="10" max="10"/>
+    <col width="19.5546875" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>VDS</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Date started</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Date Ended</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Right Sensor Activations</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Left Sensor Activations</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Feeder Sensor Activations</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Premature Responses</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Omission Responses</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Timed Responses</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Perseverant Responses</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Number of trials</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Training</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>44323.67213761574</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>44323.69326649306</v>
+      </c>
+      <c r="D2" t="n">
+        <v>44</v>
+      </c>
+      <c r="E2" t="n">
+        <v>20</v>
+      </c>
+      <c r="F2" t="n">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="G2" t="n">
+        <v>9</v>
+      </c>
+      <c r="H2" t="n">
+        <v>21</v>
+      </c>
+      <c r="I2" t="n">
+        <v>13</v>
+      </c>
+      <c r="J2" t="n">
+        <v>15</v>
+      </c>
+      <c r="K2" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Training</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>44323.70479905852</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>44323.70573404778</v>
+      </c>
+      <c r="D3" t="n">
+        <v>13</v>
+      </c>
+      <c r="E3" t="n">
+        <v>14</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>8</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>2</v>
+      </c>
+      <c r="J3" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="K3" t="n">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Final com pedidos da Madalena
</commit_message>
<xml_diff>
--- a/ratTrainer/sessions.xlsx
+++ b/ratTrainer/sessions.xlsx
@@ -15,8 +15,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -55,10 +56,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,25 +438,37 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:AA4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:K3"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="8.6640625" customWidth="1" min="1" max="1"/>
-    <col width="29.33203125" customWidth="1" min="2" max="2"/>
-    <col width="42" customWidth="1" min="3" max="3"/>
-    <col width="21.5546875" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="20.33203125" bestFit="1" customWidth="1" min="5" max="5"/>
-    <col width="22.88671875" bestFit="1" customWidth="1" min="6" max="6"/>
-    <col width="19.33203125" bestFit="1" customWidth="1" min="7" max="7"/>
-    <col width="18.109375" bestFit="1" customWidth="1" min="8" max="8"/>
-    <col width="15.5546875" bestFit="1" customWidth="1" min="9" max="9"/>
-    <col width="20.44140625" bestFit="1" customWidth="1" min="10" max="10"/>
-    <col width="19.5546875" customWidth="1" min="11" max="11"/>
+    <col width="7.44140625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="18.109375" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="18.109375" customWidth="1" min="3" max="3"/>
+    <col width="18.109375" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="21.5546875" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="20.33203125" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="22.88671875" bestFit="1" customWidth="1" min="7" max="7"/>
+    <col width="19.33203125" bestFit="1" customWidth="1" min="8" max="8"/>
+    <col width="18.109375" bestFit="1" customWidth="1" min="9" max="9"/>
+    <col width="15.5546875" bestFit="1" customWidth="1" min="10" max="10"/>
+    <col width="20.44140625" bestFit="1" customWidth="1" min="11" max="11"/>
+    <col width="7" bestFit="1" customWidth="1" min="12" max="12"/>
+    <col width="7.21875" bestFit="1" customWidth="1" min="13" max="13"/>
+    <col width="6.88671875" bestFit="1" customWidth="1" min="14" max="15"/>
+    <col width="6.5546875" bestFit="1" customWidth="1" min="16" max="16"/>
+    <col width="6.77734375" bestFit="1" customWidth="1" min="17" max="17"/>
+    <col width="6.44140625" bestFit="1" customWidth="1" min="18" max="19"/>
+    <col width="7.5546875" bestFit="1" customWidth="1" min="20" max="20"/>
+    <col width="7.77734375" bestFit="1" customWidth="1" min="21" max="21"/>
+    <col width="7.44140625" bestFit="1" customWidth="1" min="22" max="23"/>
+    <col width="7.21875" bestFit="1" customWidth="1" min="24" max="24"/>
+    <col width="7.44140625" bestFit="1" customWidth="1" min="25" max="25"/>
+    <col width="7.109375" bestFit="1" customWidth="1" min="26" max="27"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -475,42 +489,122 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Number of trials</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Right Sensor Activations</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Left Sensor Activations</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Feeder Sensor Activations</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Premature Responses</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Omission Responses</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Timed Responses</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Perseverant Responses</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Number of trials</t>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>PR - 3is</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>OR - 3is</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>TR - 3is</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>SR - 3is</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>PR - 6s</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>OR - 6s</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>TR - 6s</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>SR - 6s</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>PR - 12s</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>OR - 12s</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>TR - 12s</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>SR - 12s</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>PR - 3fs</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>OR - 3fs</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>TR - 3fs</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>SR - 3fs</t>
         </is>
       </c>
     </row>
@@ -527,28 +621,28 @@
         <v>44323.69326649306</v>
       </c>
       <c r="D2" t="n">
+        <v>43</v>
+      </c>
+      <c r="E2" t="n">
         <v>44</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>20</v>
       </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
       <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
         <v>9</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>21</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>13</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>15</v>
-      </c>
-      <c r="K2" t="n">
-        <v>43</v>
       </c>
     </row>
     <row r="3">
@@ -558,34 +652,119 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>44323.70479905852</v>
+        <v>44323.7047990625</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>44323.70573404778</v>
+        <v>44323.70573405093</v>
       </c>
       <c r="D3" t="n">
+        <v>10</v>
+      </c>
+      <c r="E3" t="n">
         <v>13</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>14</v>
       </c>
-      <c r="F3" t="n">
-        <v>0</v>
-      </c>
       <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
         <v>8</v>
       </c>
-      <c r="H3" t="n">
-        <v>0</v>
-      </c>
       <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
         <v>2</v>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>1</v>
       </c>
-      <c r="K3" t="n">
-        <v>10</v>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>44327.18941920334</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>44327.20417352678</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>120</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>120</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>25</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>34</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0</v>
+      </c>
+      <c r="U4" t="n">
+        <v>36</v>
+      </c>
+      <c r="V4" t="n">
+        <v>0</v>
+      </c>
+      <c r="W4" t="n">
+        <v>0</v>
+      </c>
+      <c r="X4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>25</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
5 seconds alert! Pequenos bugs corrigidos!
</commit_message>
<xml_diff>
--- a/ratTrainer/sessions.xlsx
+++ b/ratTrainer/sessions.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA4"/>
+  <dimension ref="A1:AA6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L1" sqref="L1"/>
@@ -689,10 +689,10 @@
         </is>
       </c>
       <c r="B4" s="3" t="n">
-        <v>44327.18941920334</v>
+        <v>44327.18941920139</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>44327.20417352678</v>
+        <v>44327.2041735301</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
@@ -764,6 +764,80 @@
         <v>0</v>
       </c>
       <c r="AA4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Training</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>44341.75635722222</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>44341.77731420139</v>
+      </c>
+      <c r="D5" t="n">
+        <v>3</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" t="n">
+        <v>3</v>
+      </c>
+      <c r="G5" t="n">
+        <v>28</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>26</v>
+      </c>
+      <c r="J5" t="n">
+        <v>2</v>
+      </c>
+      <c r="K5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Training</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>44341.79840987932</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>44341.81956005171</v>
+      </c>
+      <c r="D6" t="n">
+        <v>31</v>
+      </c>
+      <c r="E6" t="n">
+        <v>7</v>
+      </c>
+      <c r="F6" t="n">
+        <v>3</v>
+      </c>
+      <c r="G6" t="n">
+        <v>4</v>
+      </c>
+      <c r="H6" t="n">
+        <v>3</v>
+      </c>
+      <c r="I6" t="n">
+        <v>25</v>
+      </c>
+      <c r="J6" t="n">
+        <v>3</v>
+      </c>
+      <c r="K6" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>